<commit_message>
added latest WorkflowDetails.xlsx file
</commit_message>
<xml_diff>
--- a/com.automation.selenium/src/test/resources/TestData/WorkflowDetails.xlsx
+++ b/com.automation.selenium/src/test/resources/TestData/WorkflowDetails.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="6435"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="34">
   <si>
     <t>WorkflowName</t>
   </si>
@@ -30,29 +30,114 @@
     <t>zip_path</t>
   </si>
   <si>
-    <t>WF1_Set WF result</t>
-  </si>
-  <si>
-    <t>D:\Tejaswini_WF\CheckStatus.zip</t>
-  </si>
-  <si>
     <t>WF001</t>
   </si>
   <si>
     <t>TC ID</t>
   </si>
   <si>
-    <t>status completed</t>
+    <t>agentName</t>
+  </si>
+  <si>
+    <t>asd</t>
+  </si>
+  <si>
+    <t>ResultStatus</t>
+  </si>
+  <si>
+    <t>Message</t>
+  </si>
+  <si>
+    <t>status diverted</t>
+  </si>
+  <si>
+    <t>Diverted</t>
+  </si>
+  <si>
+    <t>Error! : human reason ha</t>
+  </si>
+  <si>
+    <t>Resultparam1</t>
+  </si>
+  <si>
+    <t>Resultparam2</t>
+  </si>
+  <si>
+    <t>Resultparam3</t>
+  </si>
+  <si>
+    <t>OutputTextcount</t>
+  </si>
+  <si>
+    <t>a : 75.0</t>
+  </si>
+  <si>
+    <t>Student Name : darshana</t>
+  </si>
+  <si>
+    <t>Student id : 104.0</t>
+  </si>
+  <si>
+    <t>Resultparam4</t>
+  </si>
+  <si>
+    <t>Resultparam5</t>
+  </si>
+  <si>
+    <t>Resultparam6</t>
+  </si>
+  <si>
+    <t>DivertedStatus\StudentInformation.xlsx</t>
+  </si>
+  <si>
+    <t>DivertedStatus\HindiMarks.xlsx</t>
+  </si>
+  <si>
+    <t>DivertedStatus\out.txt</t>
+  </si>
+  <si>
+    <t>WF002</t>
+  </si>
+  <si>
+    <t>DivertedStatus\DivertedStatus.zip</t>
+  </si>
+  <si>
+    <t>WF3_Set WF Diverted automation test</t>
+  </si>
+  <si>
+    <t>test\test.zip</t>
+  </si>
+  <si>
+    <t>completed test</t>
+  </si>
+  <si>
+    <t>fgh</t>
+  </si>
+  <si>
+    <t>Complete</t>
+  </si>
+  <si>
+    <t>Message : Execution Successful</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0;[Red]0"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF212529"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -78,8 +163,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -381,56 +482,209 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="23.7109375" customWidth="1"/>
-    <col min="3" max="3" width="20.5703125" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" customWidth="1"/>
-    <col min="5" max="5" width="33.5703125" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="23.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="38.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.85546875" style="4" customWidth="1"/>
+    <col min="9" max="9" width="15.140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="28.42578125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="23.5703125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="28.28515625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="18.5703125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="19.140625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="15.7109375" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" t="s">
+      <c r="G2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="5">
+        <v>6</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E3" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="F3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2">
+    <row r="4" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="1">
         <v>1</v>
       </c>
-      <c r="E2" t="s">
-        <v>5</v>
-      </c>
+      <c r="E4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H4" s="5">
+        <v>0</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J4" s="2"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -438,7 +692,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>